<commit_message>
static: static files updated
</commit_message>
<xml_diff>
--- a/static/xlsx/Aylık Plan.xlsx
+++ b/static/xlsx/Aylık Plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>Görev</t>
   </si>
@@ -25,13 +25,13 @@
     <t>Bitiş</t>
   </si>
   <si>
-    <t>Sorumlular</t>
+    <t>Kulüpler</t>
   </si>
   <si>
     <t>Detay</t>
   </si>
   <si>
-    <t>Binance ile ortak bir eğitim</t>
+    <t>Binance ile ortak eğitim</t>
   </si>
   <si>
     <t>01.07.2023</t>
@@ -46,43 +46,52 @@
     <t>Binance'in üniversiteler ekibi ile iletişime geçilip bir blockchain dalı üzerine workshop düzenlenecek</t>
   </si>
   <si>
-    <t>Sektörden bir uzman ile webinar</t>
-  </si>
-  <si>
-    <t>10.07.2023</t>
+    <t>Oyun sektöründen bir uzman ile webinar</t>
+  </si>
+  <si>
+    <t>15.07.2023</t>
+  </si>
+  <si>
+    <t>Oyun Geliştirme Kulübü</t>
+  </si>
+  <si>
+    <t>Oyun geliştirme sektöründe tecrübesi bulunan bir uzman ile webinar düzenlenecek</t>
+  </si>
+  <si>
+    <t>Kulüp YKsı ile bir eğitim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kulüp YKsının vereceği temel seviye bir oyun geliştirme eğitimi </t>
+  </si>
+  <si>
+    <t>AI sektöründen bir uzman ile webinar</t>
+  </si>
+  <si>
+    <t>Yapay Zeka Kulübü</t>
+  </si>
+  <si>
+    <t>Yapay zeka sektöründe tecrübesi bulunan bir uzman ile webinar düzenlenecek</t>
+  </si>
+  <si>
+    <t>Yapay zekanın geleceği söyleşisi</t>
+  </si>
+  <si>
+    <t>Yapay Zekanın Geleceği konusunda öğrencilerin de aktif olarak katılabileceği bir söyleşi yapılacak</t>
+  </si>
+  <si>
+    <t>Sektörden bir uzman ile eğitim</t>
+  </si>
+  <si>
+    <t>Uygulama Geliştirme Kulübü</t>
+  </si>
+  <si>
+    <t>Uygulama geliştirme sektöründe tecrübesi bulunan bir uzman ile temel seviye bir Git eğitimi düzenlenecek</t>
+  </si>
+  <si>
+    <t>Labris Network ile söyleşi</t>
   </si>
   <si>
     <t>20.07.2023</t>
-  </si>
-  <si>
-    <t>Oyun Geliştirme Kulübü</t>
-  </si>
-  <si>
-    <t>Oyun geliştirme sektöründe tecrübesi bulunan bir uzman ile webinar düzenlenecek</t>
-  </si>
-  <si>
-    <t>Yapay zekanın geleceği söyleşisi</t>
-  </si>
-  <si>
-    <t>15.07.2023</t>
-  </si>
-  <si>
-    <t>Yapay Zeka Kulübü</t>
-  </si>
-  <si>
-    <t>Yapay Zekanın Geleceği konusunda öğrencilerin de aktif olarak katılabileceği bir söyleşi yapılacak</t>
-  </si>
-  <si>
-    <t>Sektörden bir uzman ile eğitim</t>
-  </si>
-  <si>
-    <t>Uygulama Geliştirme Kulübü</t>
-  </si>
-  <si>
-    <t>Uygulama geliştirme sektöründe tecrübesi bulunan bir uzman ile temel seviye bir Git eğitimi düzenlenecek</t>
-  </si>
-  <si>
-    <t>Labris Network ile söyleşi</t>
   </si>
   <si>
     <t>Siber Güvenlik Kulübü</t>
@@ -96,10 +105,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="21">
@@ -119,8 +128,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -128,40 +175,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -173,22 +197,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -204,11 +212,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -219,8 +249,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -228,36 +267,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -272,13 +281,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -290,109 +437,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -404,55 +449,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -463,6 +472,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -505,41 +529,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -563,151 +557,166 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1040,7 +1049,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1093,74 +1102,102 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" t="s">
         <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>17</v>
+      <c r="D4" t="s">
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
         <v>23</v>
       </c>
-      <c r="E6" t="s">
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="4:4">
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="4:4">
-      <c r="D8" s="5"/>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="4:4">
       <c r="D9" s="5"/>

</xml_diff>

<commit_message>
feature: aylık planlar changed to proje planları
</commit_message>
<xml_diff>
--- a/static/xlsx/Aylık Plan.xlsx
+++ b/static/xlsx/Aylık Plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Görev</t>
   </si>
@@ -31,73 +31,40 @@
     <t>Detay</t>
   </si>
   <si>
-    <t>Binance ile ortak eğitim</t>
-  </si>
-  <si>
-    <t>01.07.2023</t>
-  </si>
-  <si>
-    <t>01.08.2023</t>
-  </si>
-  <si>
-    <t>Blockchain Kulübü</t>
-  </si>
-  <si>
-    <t>Binance'in üniversiteler ekibi ile iletişime geçilip bir blockchain dalı üzerine workshop düzenlenecek</t>
-  </si>
-  <si>
-    <t>Oyun sektöründen bir uzman ile webinar</t>
-  </si>
-  <si>
-    <t>15.07.2023</t>
-  </si>
-  <si>
-    <t>Oyun Geliştirme Kulübü</t>
-  </si>
-  <si>
-    <t>Oyun geliştirme sektöründe tecrübesi bulunan bir uzman ile webinar düzenlenecek</t>
-  </si>
-  <si>
-    <t>Kulüp YKsı ile bir eğitim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kulüp YKsının vereceği temel seviye bir oyun geliştirme eğitimi </t>
-  </si>
-  <si>
-    <t>AI sektöründen bir uzman ile webinar</t>
+    <t>TestGPT</t>
+  </si>
+  <si>
+    <t>01.10.2023</t>
+  </si>
+  <si>
+    <t>31.12.2023</t>
   </si>
   <si>
     <t>Yapay Zeka Kulübü</t>
   </si>
   <si>
-    <t>Yapay zeka sektöründe tecrübesi bulunan bir uzman ile webinar düzenlenecek</t>
-  </si>
-  <si>
-    <t>Yapay zekanın geleceği söyleşisi</t>
-  </si>
-  <si>
-    <t>Yapay Zekanın Geleceği konusunda öğrencilerin de aktif olarak katılabileceği bir söyleşi yapılacak</t>
-  </si>
-  <si>
-    <t>Sektörden bir uzman ile eğitim</t>
+    <t>Herhangi bir konuyu daha hızlı öğrenmeyi sağlayacak yapay zekalı bir sohbet botu</t>
+  </si>
+  <si>
+    <t>Kulüp Web Sayfaları</t>
+  </si>
+  <si>
+    <t>31.10.2023</t>
   </si>
   <si>
     <t>Uygulama Geliştirme Kulübü</t>
   </si>
   <si>
-    <t>Uygulama geliştirme sektöründe tecrübesi bulunan bir uzman ile temel seviye bir Git eğitimi düzenlenecek</t>
-  </si>
-  <si>
-    <t>Labris Network ile söyleşi</t>
-  </si>
-  <si>
-    <t>20.07.2023</t>
-  </si>
-  <si>
-    <t>Siber Güvenlik Kulübü</t>
-  </si>
-  <si>
-    <t>Labris Network ile siber güvenlik alanındaki fırsatların konuşulacağı bir söyleşi</t>
+    <t>Topluluk altındaki alt kulüplerin kendi web sayfaları</t>
+  </si>
+  <si>
+    <t>Insta ve Medium Botları</t>
+  </si>
+  <si>
+    <t>01.11.2023</t>
+  </si>
+  <si>
+    <t>Instagram ve Mediumdaki sosyal medya yönetimini otomatize edecek botlar</t>
   </si>
 </sst>
 </file>
@@ -105,10 +72,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="21">
@@ -129,12 +96,36 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -152,30 +143,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -190,21 +173,6 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -212,9 +180,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -222,6 +189,20 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -229,44 +210,30 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -281,19 +248,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -311,73 +404,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -389,79 +416,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -472,6 +439,32 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -490,17 +483,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -524,15 +511,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
@@ -543,17 +521,6 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -575,7 +542,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -593,130 +560,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1049,7 +1016,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1119,7 +1086,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -1128,76 +1095,20 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
-      </c>
+    </row>
+    <row r="5" spans="4:4">
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="4:4">
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="4:4">
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="4:4">
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="4:4">
       <c r="D9" s="5"/>

</xml_diff>

<commit_message>
refactor: date columnd deleted for load_excel uploading plan, create_schema moved to utils
</commit_message>
<xml_diff>
--- a/static/xlsx/Aylık Plan.xlsx
+++ b/static/xlsx/Aylık Plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Görev</t>
   </si>
@@ -34,12 +34,6 @@
     <t>Community Website Updates</t>
   </si>
   <si>
-    <t>01.10.2023</t>
-  </si>
-  <si>
-    <t>31.10.2023</t>
-  </si>
-  <si>
     <t>Uygulama Geliştirme Kulübü</t>
   </si>
   <si>
@@ -49,12 +43,6 @@
     <t>News Craft</t>
   </si>
   <si>
-    <t>01.11.2023</t>
-  </si>
-  <si>
-    <t>30.11.2023</t>
-  </si>
-  <si>
     <t xml:space="preserve">Yapay Zeka Kulübü </t>
   </si>
   <si>
@@ -62,12 +50,6 @@
   </si>
   <si>
     <t>Social Master</t>
-  </si>
-  <si>
-    <t>01.12.2023</t>
-  </si>
-  <si>
-    <t>31.12.2023</t>
   </si>
   <si>
     <t>Instagram ve Mediumdaki sosyal medya yönetimini otomatize edecek botlar</t>
@@ -693,12 +675,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1022,7 +1003,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1057,142 +1038,142 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1">
+        <v>45200</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45230</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45231</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45260</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45261</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45291</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="4:4">
-      <c r="D5" s="5"/>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="4:4">
-      <c r="D6" s="5"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="4:4">
-      <c r="D7" s="5"/>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" spans="4:4">
-      <c r="D8" s="5"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="4:4">
-      <c r="D9" s="5"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="4:4">
-      <c r="D10" s="5"/>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="4:4">
-      <c r="D11" s="5"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="4:4">
-      <c r="D12" s="5"/>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" spans="4:4">
-      <c r="D13" s="5"/>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="4:4">
-      <c r="D14" s="5"/>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="4:4">
-      <c r="D15" s="5"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="4:4">
-      <c r="D16" s="5"/>
+      <c r="D16" s="4"/>
     </row>
     <row r="17" spans="4:4">
-      <c r="D17" s="5"/>
+      <c r="D17" s="4"/>
     </row>
     <row r="18" spans="4:4">
-      <c r="D18" s="5"/>
+      <c r="D18" s="4"/>
     </row>
     <row r="19" spans="4:4">
-      <c r="D19" s="5"/>
+      <c r="D19" s="4"/>
     </row>
     <row r="20" spans="4:4">
-      <c r="D20" s="5"/>
+      <c r="D20" s="4"/>
     </row>
     <row r="21" spans="4:4">
-      <c r="D21" s="5"/>
+      <c r="D21" s="4"/>
     </row>
     <row r="22" spans="4:4">
-      <c r="D22" s="5"/>
+      <c r="D22" s="4"/>
     </row>
     <row r="23" spans="4:4">
-      <c r="D23" s="5"/>
+      <c r="D23" s="4"/>
     </row>
     <row r="24" spans="4:4">
-      <c r="D24" s="5"/>
+      <c r="D24" s="4"/>
     </row>
     <row r="25" spans="4:4">
-      <c r="D25" s="5"/>
+      <c r="D25" s="4"/>
     </row>
     <row r="26" spans="4:4">
-      <c r="D26" s="5"/>
+      <c r="D26" s="4"/>
     </row>
     <row r="27" spans="4:4">
-      <c r="D27" s="5"/>
+      <c r="D27" s="4"/>
     </row>
     <row r="28" spans="4:4">
-      <c r="D28" s="5"/>
+      <c r="D28" s="4"/>
     </row>
     <row r="29" spans="4:4">
-      <c r="D29" s="5"/>
+      <c r="D29" s="4"/>
     </row>
     <row r="30" spans="4:4">
-      <c r="D30" s="5"/>
+      <c r="D30" s="4"/>
     </row>
     <row r="31" spans="4:4">
-      <c r="D31" s="5"/>
+      <c r="D31" s="4"/>
     </row>
     <row r="32" spans="4:4">
-      <c r="D32" s="5"/>
+      <c r="D32" s="4"/>
     </row>
     <row r="33" spans="4:4">
-      <c r="D33" s="5"/>
+      <c r="D33" s="4"/>
     </row>
     <row r="34" spans="4:4">
-      <c r="D34" s="5"/>
+      <c r="D34" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>